<commit_message>
FIxed issues in bulk upload storage
</commit_message>
<xml_diff>
--- a/public/files/storages/Storage_Bulk_Upload_Excel_Format.xlsx
+++ b/public/files/storages/Storage_Bulk_Upload_Excel_Format.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>Sample Code</t>
   </si>
@@ -33,24 +33,6 @@
   </si>
   <si>
     <t>Volume (ml)</t>
-  </si>
-  <si>
-    <t>VL08220003</t>
-  </si>
-  <si>
-    <t>VL08220004</t>
-  </si>
-  <si>
-    <t>VL08220005</t>
-  </si>
-  <si>
-    <t>VL08220006</t>
-  </si>
-  <si>
-    <t>VL09220007</t>
-  </si>
-  <si>
-    <t>VL09220008</t>
   </si>
 </sst>
 </file>
@@ -445,7 +427,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ7"/>
+  <dimension ref="A1:AMJ1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1504,36 +1486,6 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:1024">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1024">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1024">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1024">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1024">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1024">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7875" right="0.7875" top="1.0527777777778" bottom="1.0527777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added clear option for sample test date in test result report filter
</commit_message>
<xml_diff>
--- a/public/files/storages/Storage_Bulk_Upload_Excel_Format.xlsx
+++ b/public/files/storages/Storage_Bulk_Upload_Excel_Format.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Sample Code</t>
   </si>
@@ -33,6 +33,21 @@
   </si>
   <si>
     <t>Volume (ml)</t>
+  </si>
+  <si>
+    <t>VL042284501</t>
+  </si>
+  <si>
+    <t>VL042284502</t>
+  </si>
+  <si>
+    <t>VL042284512</t>
+  </si>
+  <si>
+    <t>VL042284513</t>
+  </si>
+  <si>
+    <t>VL0822020</t>
   </si>
 </sst>
 </file>
@@ -427,7 +442,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1"/>
+  <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1486,6 +1501,31 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
+    <row r="2" spans="1:1024">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1024">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1024">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1024">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1024">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7875" right="0.7875" top="1.0527777777778" bottom="1.0527777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added patient id column in bulk upload storage template file
</commit_message>
<xml_diff>
--- a/public/files/storages/Storage_Bulk_Upload_Excel_Format.xlsx
+++ b/public/files/storages/Storage_Bulk_Upload_Excel_Format.xlsx
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>Sample Code</t>
+  </si>
+  <si>
+    <t>Patient ID</t>
   </si>
   <si>
     <t>Feezer Code</t>
@@ -33,21 +36,6 @@
   </si>
   <si>
     <t>Volume (ml)</t>
-  </si>
-  <si>
-    <t>VL042284501</t>
-  </si>
-  <si>
-    <t>VL042284502</t>
-  </si>
-  <si>
-    <t>VL042284512</t>
-  </si>
-  <si>
-    <t>VL042284513</t>
-  </si>
-  <si>
-    <t>VL0822020</t>
   </si>
 </sst>
 </file>
@@ -442,7 +430,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ6"/>
+  <dimension ref="A1:AMJ1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A1">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +439,17 @@
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="23.6875" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="36.84" customWidth="true" style="1"/>
-    <col min="2" max="2" width="16.48" customWidth="true" style="1"/>
-    <col min="3" max="3" width="22.33" customWidth="true" style="1"/>
-    <col min="4" max="4" width="16" customWidth="true" style="1"/>
-    <col min="5" max="5" width="16.48" customWidth="true" style="1"/>
-    <col min="6" max="6" width="42.52" customWidth="true" style="1"/>
-    <col min="7" max="7" width="28.33" customWidth="true" style="1"/>
-    <col min="8" max="8" width="18.85" customWidth="true" style="1"/>
-    <col min="9" max="9" width="21.33" customWidth="true" style="1"/>
-    <col min="10" max="10" width="15.49" customWidth="true" style="1"/>
-    <col min="11" max="11" width="17" customWidth="true" style="1"/>
-    <col min="12" max="12" width="23.66" customWidth="true" style="1"/>
+    <col min="2" max="2" width="21.95" customWidth="true" style="1"/>
+    <col min="3" max="3" width="16.48" customWidth="true" style="1"/>
+    <col min="4" max="4" width="22.33" customWidth="true" style="1"/>
+    <col min="5" max="5" width="16" customWidth="true" style="1"/>
+    <col min="6" max="6" width="16.48" customWidth="true" style="1"/>
+    <col min="7" max="7" width="42.52" customWidth="true" style="1"/>
+    <col min="8" max="8" width="28.33" customWidth="true" style="1"/>
+    <col min="9" max="9" width="18.85" customWidth="true" style="1"/>
+    <col min="10" max="10" width="21.33" customWidth="true" style="1"/>
+    <col min="11" max="11" width="15.49" customWidth="true" style="1"/>
+    <col min="12" max="12" width="17" customWidth="true" style="1"/>
     <col min="13" max="13" width="23.66" customWidth="true" style="1"/>
     <col min="14" max="14" width="23.66" customWidth="true" style="1"/>
     <col min="15" max="15" width="23.66" customWidth="true" style="1"/>
@@ -1480,7 +1468,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1495,36 +1483,14 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:1024">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1024">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1024">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1024">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1024">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="L1" s="3"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>